<commit_message>
tăng kích thước cỡ chữ chat của UI
</commit_message>
<xml_diff>
--- a/src/back-end/backend_vector_database/dataset/LegalRAG.xlsx
+++ b/src/back-end/backend_vector_database/dataset/LegalRAG.xlsx
@@ -1326,19 +1326,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1374,7 +1368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1385,11 +1379,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1699,32 +1690,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="37.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="107.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="37.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="107.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
@@ -1759,11 +1750,11 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="639.75" customFormat="1" s="1">
-      <c r="A2" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="618" customFormat="1" s="1">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3"/>
@@ -1792,10 +1783,10 @@
       <c r="Z2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="666" customFormat="1" s="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3"/>
@@ -1824,10 +1815,10 @@
       <c r="Z3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="573.75" customFormat="1" s="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3"/>
@@ -1856,10 +1847,10 @@
       <c r="Z4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="705.75" customFormat="1" s="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3"/>
@@ -1888,10 +1879,10 @@
       <c r="Z5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="480.75" customFormat="1" s="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3"/>
@@ -1920,10 +1911,10 @@
       <c r="Z6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="480.75" customFormat="1" s="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3"/>
@@ -1952,10 +1943,10 @@
       <c r="Z7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="494.25" customFormat="1" s="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3"/>
@@ -1984,10 +1975,10 @@
       <c r="Z8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="428.25" customFormat="1" s="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="3"/>
@@ -2016,10 +2007,10 @@
       <c r="Z9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="309.75" customFormat="1" s="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3"/>
@@ -2048,10 +2039,10 @@
       <c r="Z10" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="336" customFormat="1" s="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3"/>
@@ -2080,10 +2071,10 @@
       <c r="Z11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="375.75" customFormat="1" s="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="3"/>
@@ -2112,10 +2103,10 @@
       <c r="Z12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="3"/>
@@ -2144,10 +2135,10 @@
       <c r="Z13" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="3"/>
@@ -2176,10 +2167,10 @@
       <c r="Z14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="3"/>
@@ -2208,10 +2199,10 @@
       <c r="Z15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="3"/>
@@ -2240,10 +2231,10 @@
       <c r="Z16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="3"/>
@@ -2272,10 +2263,10 @@
       <c r="Z17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="3"/>
@@ -2304,10 +2295,10 @@
       <c r="Z18" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="3"/>
@@ -2336,10 +2327,10 @@
       <c r="Z19" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="3"/>
@@ -2368,10 +2359,10 @@
       <c r="Z20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="3"/>
@@ -2400,10 +2391,10 @@
       <c r="Z21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="3"/>
@@ -2432,10 +2423,10 @@
       <c r="Z22" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="3"/>
@@ -2464,10 +2455,10 @@
       <c r="Z23" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="3"/>
@@ -2496,10 +2487,10 @@
       <c r="Z24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="3"/>
@@ -2528,10 +2519,10 @@
       <c r="Z25" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="3"/>
@@ -2560,10 +2551,10 @@
       <c r="Z26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="3"/>
@@ -2592,10 +2583,10 @@
       <c r="Z27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="3"/>
@@ -2624,10 +2615,10 @@
       <c r="Z28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="3"/>
@@ -2656,10 +2647,10 @@
       <c r="Z29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="3"/>
@@ -2688,10 +2679,10 @@
       <c r="Z30" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="3"/>
@@ -2720,10 +2711,10 @@
       <c r="Z31" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C32" s="3"/>
@@ -2752,10 +2743,10 @@
       <c r="Z32" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="3"/>
@@ -2784,10 +2775,10 @@
       <c r="Z33" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="3"/>
@@ -2816,10 +2807,10 @@
       <c r="Z34" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C35" s="3"/>
@@ -2848,10 +2839,10 @@
       <c r="Z35" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="3"/>
@@ -2880,10 +2871,10 @@
       <c r="Z36" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C37" s="3"/>
@@ -2912,10 +2903,10 @@
       <c r="Z37" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="3"/>
@@ -2944,10 +2935,10 @@
       <c r="Z38" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C39" s="3"/>
@@ -2976,10 +2967,10 @@
       <c r="Z39" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C40" s="3"/>
@@ -3008,10 +2999,10 @@
       <c r="Z40" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C41" s="3"/>
@@ -3040,10 +3031,10 @@
       <c r="Z41" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C42" s="3"/>
@@ -3072,10 +3063,10 @@
       <c r="Z42" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="3"/>
@@ -3104,10 +3095,10 @@
       <c r="Z43" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C44" s="3"/>
@@ -3136,10 +3127,10 @@
       <c r="Z44" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="3"/>
@@ -3168,10 +3159,10 @@
       <c r="Z45" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C46" s="3"/>
@@ -3200,10 +3191,10 @@
       <c r="Z46" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C47" s="3"/>
@@ -3232,10 +3223,10 @@
       <c r="Z47" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C48" s="3"/>
@@ -3264,10 +3255,10 @@
       <c r="Z48" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C49" s="3"/>
@@ -3296,10 +3287,10 @@
       <c r="Z49" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="3"/>
@@ -3328,10 +3319,10 @@
       <c r="Z50" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C51" s="3"/>
@@ -3360,10 +3351,10 @@
       <c r="Z51" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C52" s="3"/>
@@ -3392,10 +3383,10 @@
       <c r="Z52" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>105</v>
       </c>
       <c r="C53" s="3"/>
@@ -3424,10 +3415,10 @@
       <c r="Z53" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C54" s="3"/>
@@ -3456,10 +3447,10 @@
       <c r="Z54" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C55" s="3"/>
@@ -3488,10 +3479,10 @@
       <c r="Z55" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C56" s="3"/>
@@ -3520,10 +3511,10 @@
       <c r="Z56" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C57" s="3"/>
@@ -3552,10 +3543,10 @@
       <c r="Z57" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C58" s="3"/>
@@ -3584,10 +3575,10 @@
       <c r="Z58" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C59" s="3"/>
@@ -3616,10 +3607,10 @@
       <c r="Z59" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C60" s="3"/>
@@ -3648,10 +3639,10 @@
       <c r="Z60" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C61" s="3"/>
@@ -3680,10 +3671,10 @@
       <c r="Z61" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C62" s="3"/>
@@ -3712,10 +3703,10 @@
       <c r="Z62" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C63" s="3"/>
@@ -3744,10 +3735,10 @@
       <c r="Z63" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C64" s="3"/>
@@ -3776,10 +3767,10 @@
       <c r="Z64" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C65" s="3"/>
@@ -3808,10 +3799,10 @@
       <c r="Z65" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C66" s="3"/>
@@ -3840,10 +3831,10 @@
       <c r="Z66" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C67" s="3"/>
@@ -3872,10 +3863,10 @@
       <c r="Z67" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C68" s="3"/>
@@ -3904,10 +3895,10 @@
       <c r="Z68" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C69" s="3"/>
@@ -3936,10 +3927,10 @@
       <c r="Z69" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C70" s="3"/>
@@ -3968,10 +3959,10 @@
       <c r="Z70" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C71" s="3"/>
@@ -4000,10 +3991,10 @@
       <c r="Z71" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>143</v>
       </c>
       <c r="C72" s="3"/>
@@ -4032,10 +4023,10 @@
       <c r="Z72" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>145</v>
       </c>
       <c r="C73" s="3"/>
@@ -4064,10 +4055,10 @@
       <c r="Z73" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>147</v>
       </c>
       <c r="C74" s="3"/>
@@ -4096,10 +4087,10 @@
       <c r="Z74" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>149</v>
       </c>
       <c r="C75" s="3"/>
@@ -4128,10 +4119,10 @@
       <c r="Z75" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C76" s="3"/>
@@ -4160,10 +4151,10 @@
       <c r="Z76" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>153</v>
       </c>
       <c r="C77" s="3"/>
@@ -4192,10 +4183,10 @@
       <c r="Z77" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C78" s="3"/>
@@ -4224,10 +4215,10 @@
       <c r="Z78" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>157</v>
       </c>
       <c r="C79" s="3"/>
@@ -4256,10 +4247,10 @@
       <c r="Z79" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C80" s="3"/>
@@ -4288,10 +4279,10 @@
       <c r="Z80" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C81" s="3"/>
@@ -4320,10 +4311,10 @@
       <c r="Z81" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>163</v>
       </c>
       <c r="C82" s="3"/>
@@ -4352,10 +4343,10 @@
       <c r="Z82" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>165</v>
       </c>
       <c r="C83" s="3"/>
@@ -4384,10 +4375,10 @@
       <c r="Z83" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C84" s="3"/>
@@ -4416,10 +4407,10 @@
       <c r="Z84" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C85" s="3"/>
@@ -4448,10 +4439,10 @@
       <c r="Z85" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>171</v>
       </c>
       <c r="C86" s="3"/>

</xml_diff>